<commit_message>
replace font in xlsx workbook
</commit_message>
<xml_diff>
--- a/evap/static/sample.xlsx
+++ b/evap/static/sample.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="MA Belegungen" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="BA Belegungen" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MA Belegungen" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="BA Belegungen" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn__FilterDatabase" vbProcedure="false">'MA Belegungen'!$A$1:$K$22</definedName>
@@ -132,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,19 +154,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -224,40 +211,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -273,63 +244,170 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="17.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -337,38 +415,37 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -384,104 +461,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="17.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replace font in xlsx workbook (#2218)
</commit_message>
<xml_diff>
--- a/evap/static/sample.xlsx
+++ b/evap/static/sample.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="MA Belegungen" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="BA Belegungen" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="MA Belegungen" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="BA Belegungen" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn__FilterDatabase" vbProcedure="false">'MA Belegungen'!$A$1:$K$22</definedName>
@@ -132,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,19 +154,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -224,40 +211,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -273,63 +244,170 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="17.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -337,38 +415,37 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -384,104 +461,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="17.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>